<commit_message>
Created MOE education cluster mapping
</commit_message>
<xml_diff>
--- a/data/graduate-employment-survey-ntu-nus-sit-smu-suss-sutd.xlsx
+++ b/data/graduate-employment-survey-ntu-nus-sit-smu-suss-sutd.xlsx
@@ -1,26 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Desktop\MTech EBAC Sem 1\Practice Module\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Desktop\MTech EBAC Sem 1\Practice Module\F5-APM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AAD6709B-F33B-421E-BD20-476B96B94114}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6F2F4D-2E94-490E-8166-60421E703367}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1326" yWindow="0" windowWidth="17340" windowHeight="10200"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="graduate-employment-survey-ntu-" sheetId="1" r:id="rId1"/>
+    <sheet name="course-cluster" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'graduate-employment-survey-ntu-'!$A$1:$L$704</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2705" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3116" uniqueCount="427">
   <si>
     <t>year</t>
   </si>
@@ -1076,12 +1091,238 @@
   </si>
   <si>
     <t>Bachelor of Science in Marketing</t>
+  </si>
+  <si>
+    <t>Course_Name</t>
+  </si>
+  <si>
+    <t>Cluster</t>
+  </si>
+  <si>
+    <t>Arts, Design &amp; Media</t>
+  </si>
+  <si>
+    <t>Bachelor of Engineering with Honours in Civil Engineering</t>
+  </si>
+  <si>
+    <t>Double Degree in Bachelor of Engineering (Hons) (Civil Engineering) and Bachelor of Arts (Hons) in Economics</t>
+  </si>
+  <si>
+    <t>Bachelor of Engineering with Honours in Sustainable Infrastructure Engineering (Building Services)</t>
+  </si>
+  <si>
+    <t>Built Environment</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Supply Chain Management</t>
+  </si>
+  <si>
+    <t>University</t>
+  </si>
+  <si>
+    <t>Bachelor of Social Sciences (majors in Theatre Studies and Communications and New Media)</t>
+  </si>
+  <si>
+    <t>NUS</t>
+  </si>
+  <si>
+    <t>NTU</t>
+  </si>
+  <si>
+    <t>SIT</t>
+  </si>
+  <si>
+    <t>Bachelor of Arts (Architecture)</t>
+  </si>
+  <si>
+    <t>Bachelor of Science (Architecture and Sustainable Design)</t>
+  </si>
+  <si>
+    <t>SUTD</t>
+  </si>
+  <si>
+    <t>Bachelor of Business Management</t>
+  </si>
+  <si>
+    <t>SMU</t>
+  </si>
+  <si>
+    <t>Bachelor of Human Resource Management</t>
+  </si>
+  <si>
+    <t>SUSS</t>
+  </si>
+  <si>
+    <t>Engineering</t>
+  </si>
+  <si>
+    <t>Double Degree in Bachelor of Engineering (Hons) (Aerospace Engineering) and Bachelor of Arts (Hons) in Economics</t>
+  </si>
+  <si>
+    <t>Bachelor of Engineering (Hons) (Chemical and Biomolecular Engineering)</t>
+  </si>
+  <si>
+    <t>Double Degree in Bachelor of Engineering (Hons) (Chemical and Biomolecular Engineering) and Bachelor of Arts (Hons) in Economics</t>
+  </si>
+  <si>
+    <t>Bachelor of Engineering (Hons) (Electrical and Electronic Engineering)</t>
+  </si>
+  <si>
+    <t>Bachelor of Engineering (Hons) (Information Engineering and Media)</t>
+  </si>
+  <si>
+    <t>Double Degree in Bachelor of Engineering (Hons) (Materials Engineering) and Bachelor of Arts (Hons) in Economics</t>
+  </si>
+  <si>
+    <t>Double Degree in Bachelor of Engineering (Hons) (Electrical and Electronic Engineering) and Bachelor of Arts (Hons) in Economics</t>
+  </si>
+  <si>
+    <t>Bachelor of Engineering with Honours in Systems Engineering (ElectroMechanical Systems)</t>
+  </si>
+  <si>
+    <t>Bachelor of Engineering with Honours in Telematics (Intelligent Transportation Systems Engineering)</t>
+  </si>
+  <si>
+    <t>Bachelor of Engineering with Honours in Pharmaceutical Engineering</t>
+  </si>
+  <si>
+    <t>Bachelor of Food Technology with Honours</t>
+  </si>
+  <si>
+    <t>Health Sciences</t>
+  </si>
+  <si>
+    <t>Bachelor of Science (Pharmacy)</t>
+  </si>
+  <si>
+    <t>Bachelor in Science with Honours (Occupational Therapy)</t>
+  </si>
+  <si>
+    <t>Bachelor in Science with Honours (Physiotherapy)</t>
+  </si>
+  <si>
+    <t>Bachelor in Science with Honours (Diagnostic Radiography)</t>
+  </si>
+  <si>
+    <t>Bachelor in Science with Honours (Radiation Therapy)</t>
+  </si>
+  <si>
+    <t>Sciences</t>
+  </si>
+  <si>
+    <t>Bachelor of Social Science</t>
+  </si>
+  <si>
+    <t>Bachelor of Social Work</t>
+  </si>
+  <si>
+    <t>Humanities &amp; Social Sciences</t>
+  </si>
+  <si>
+    <t>Bachelor of Arts (excluding majors in Theatre Studies and Communications &amp; New Media)</t>
+  </si>
+  <si>
+    <t>Bachelor of Arts (Hons) (excluding majors in Theatre Studies and Communications &amp; New Media)</t>
+  </si>
+  <si>
+    <t>Bachelor of Environmental Studies (specialisation in Environmental Geography)</t>
+  </si>
+  <si>
+    <t>Bachelor of Social Sciences (excluding majors in Theatre Studies and Communications &amp; New Media)</t>
+  </si>
+  <si>
+    <t>Bachelor of Arts (Hons) in Linguistics and Multilingual Studies</t>
+  </si>
+  <si>
+    <t>Bachelor of Arts (Hons) in Philosophy</t>
+  </si>
+  <si>
+    <t>Bachelor of Arts (Hons) in Public Policy and Global Affairs</t>
+  </si>
+  <si>
+    <t>Bachelor of Science (Hons) (Sport Science and Management)</t>
+  </si>
+  <si>
+    <t>Double Major in Bachelor of Arts (Hons) in English Literature and Art History</t>
+  </si>
+  <si>
+    <t>Double Major in Bachelor of Arts (Hons) in Psychology and Linguistics &amp; Multilingual Studies</t>
+  </si>
+  <si>
+    <t>Double Major in Bachelor of Arts (Hons) in Economics and Psychology</t>
+  </si>
+  <si>
+    <t>Double Major in Bachelor of Arts (Hons) in Economics and Public Policy &amp; Global Affairs</t>
+  </si>
+  <si>
+    <t>Double Major in Bachelor of Arts (Hons) in Psychology and Media Analytics</t>
+  </si>
+  <si>
+    <t>Bachelor of Science (Economics)</t>
+  </si>
+  <si>
+    <t>Bachelor of Early Childhood Education</t>
+  </si>
+  <si>
+    <t>Information &amp; Digital Technologies</t>
+  </si>
+  <si>
+    <t>Bachelor of Computing (Information Security)</t>
+  </si>
+  <si>
+    <t>Bachelor of Science (Data Science and Analytics)</t>
+  </si>
+  <si>
+    <t>Double Degree in Bachelor of Business (Hons) and Bachelor of Engineering (Hons) (Computer Engineering)</t>
+  </si>
+  <si>
+    <t>Double Degree in Bachelor of Engineering (Hons) (Computer Science) and Bachelor of Arts (Hons) in Economics</t>
+  </si>
+  <si>
+    <t>Bachelor of Science (Information Systems)</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Computer Science in RealTime Interactive Simulation</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Computer Science and Game Design</t>
+  </si>
+  <si>
+    <t>Bachelor of Engineering in Information and Communications Technology (Software Engineering)</t>
+  </si>
+  <si>
+    <t>Bachelor of Engineering in Information and Communications Technology
+(Information Security)</t>
+  </si>
+  <si>
+    <t>Bachelor of Science (Computational Biology)</t>
+  </si>
+  <si>
+    <t>Bachelor of Environmental Studies (specialisation in Environmental Biology)</t>
+  </si>
+  <si>
+    <t>Bachelor of Science (Hons) in Chemistry and Biological Chemistry</t>
+  </si>
+  <si>
+    <t>Bachelor of Science (Hons) in Mathematics and Economics</t>
+  </si>
+  <si>
+    <t>Bachelor of Science (Hons) in Physics and Applied Physics</t>
+  </si>
+  <si>
+    <t>Bachelor of Science (Hons) in Biomedical Sciences</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Environmental Earth Systems Science (Hons)</t>
+  </si>
+  <si>
+    <t>Double Degree in Bachelor of Science (Hons) in Biomedical Sciences and Bachelor of Medicine (Chinese Medicine)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1559,8 +1800,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1915,12 +2158,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L704"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="17.26171875" customWidth="1"/>
+    <col min="3" max="3" width="30.05078125" customWidth="1"/>
+    <col min="4" max="4" width="45.26171875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
@@ -28675,6 +28925,1534 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L704" xr:uid="{5F12A534-508F-4842-9449-EE977A6E8BFF}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FA72D28-2FCD-4EB8-BE34-CC1FA790ADCF}">
+  <dimension ref="A1:C137"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C128" sqref="C128"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="27.578125" customWidth="1"/>
+    <col min="2" max="2" width="14.47265625" customWidth="1"/>
+    <col min="3" max="3" width="52.578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>354</v>
+      </c>
+      <c r="B3" t="s">
+        <v>362</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>354</v>
+      </c>
+      <c r="B4" t="s">
+        <v>362</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>354</v>
+      </c>
+      <c r="B5" t="s">
+        <v>362</v>
+      </c>
+      <c r="C5" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>354</v>
+      </c>
+      <c r="B6" t="s">
+        <v>363</v>
+      </c>
+      <c r="C6" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>354</v>
+      </c>
+      <c r="B7" t="s">
+        <v>363</v>
+      </c>
+      <c r="C7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>354</v>
+      </c>
+      <c r="B8" t="s">
+        <v>364</v>
+      </c>
+      <c r="C8" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>354</v>
+      </c>
+      <c r="B9" t="s">
+        <v>364</v>
+      </c>
+      <c r="C9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>354</v>
+      </c>
+      <c r="B10" t="s">
+        <v>364</v>
+      </c>
+      <c r="C10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>354</v>
+      </c>
+      <c r="B11" t="s">
+        <v>364</v>
+      </c>
+      <c r="C11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>358</v>
+      </c>
+      <c r="B12" t="s">
+        <v>362</v>
+      </c>
+      <c r="C12" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>358</v>
+      </c>
+      <c r="B13" t="s">
+        <v>362</v>
+      </c>
+      <c r="C13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>358</v>
+      </c>
+      <c r="B14" t="s">
+        <v>362</v>
+      </c>
+      <c r="C14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>358</v>
+      </c>
+      <c r="B15" t="s">
+        <v>362</v>
+      </c>
+      <c r="C15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>358</v>
+      </c>
+      <c r="B16" t="s">
+        <v>363</v>
+      </c>
+      <c r="C16" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>358</v>
+      </c>
+      <c r="B17" t="s">
+        <v>363</v>
+      </c>
+      <c r="C17" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>358</v>
+      </c>
+      <c r="B18" t="s">
+        <v>367</v>
+      </c>
+      <c r="C18" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>358</v>
+      </c>
+      <c r="B19" t="s">
+        <v>364</v>
+      </c>
+      <c r="C19" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>358</v>
+      </c>
+      <c r="B20" t="s">
+        <v>364</v>
+      </c>
+      <c r="C20" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>219</v>
+      </c>
+      <c r="B21" t="s">
+        <v>362</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>219</v>
+      </c>
+      <c r="B22" t="s">
+        <v>362</v>
+      </c>
+      <c r="C22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>219</v>
+      </c>
+      <c r="B23" t="s">
+        <v>362</v>
+      </c>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>219</v>
+      </c>
+      <c r="B24" t="s">
+        <v>362</v>
+      </c>
+      <c r="C24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>219</v>
+      </c>
+      <c r="B25" t="s">
+        <v>363</v>
+      </c>
+      <c r="C25" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>219</v>
+      </c>
+      <c r="B26" t="s">
+        <v>363</v>
+      </c>
+      <c r="C26" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>219</v>
+      </c>
+      <c r="B27" t="s">
+        <v>363</v>
+      </c>
+      <c r="C27" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>219</v>
+      </c>
+      <c r="B28" t="s">
+        <v>363</v>
+      </c>
+      <c r="C28" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>219</v>
+      </c>
+      <c r="B29" t="s">
+        <v>369</v>
+      </c>
+      <c r="C29" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>219</v>
+      </c>
+      <c r="B30" t="s">
+        <v>369</v>
+      </c>
+      <c r="C30" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
+        <v>219</v>
+      </c>
+      <c r="B31" t="s">
+        <v>364</v>
+      </c>
+      <c r="C31" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>219</v>
+      </c>
+      <c r="B32" t="s">
+        <v>364</v>
+      </c>
+      <c r="C32" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>219</v>
+      </c>
+      <c r="B33" t="s">
+        <v>364</v>
+      </c>
+      <c r="C33" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>219</v>
+      </c>
+      <c r="B34" t="s">
+        <v>364</v>
+      </c>
+      <c r="C34" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>219</v>
+      </c>
+      <c r="B35" t="s">
+        <v>371</v>
+      </c>
+      <c r="C35" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>219</v>
+      </c>
+      <c r="B36" t="s">
+        <v>371</v>
+      </c>
+      <c r="C36" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>219</v>
+      </c>
+      <c r="B37" t="s">
+        <v>371</v>
+      </c>
+      <c r="C37" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>219</v>
+      </c>
+      <c r="B38" t="s">
+        <v>371</v>
+      </c>
+      <c r="C38" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>219</v>
+      </c>
+      <c r="B39" t="s">
+        <v>371</v>
+      </c>
+      <c r="C39" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>372</v>
+      </c>
+      <c r="B40" t="s">
+        <v>362</v>
+      </c>
+      <c r="C40" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>372</v>
+      </c>
+      <c r="B41" t="s">
+        <v>362</v>
+      </c>
+      <c r="C41" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>372</v>
+      </c>
+      <c r="B42" t="s">
+        <v>362</v>
+      </c>
+      <c r="C42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>372</v>
+      </c>
+      <c r="B43" t="s">
+        <v>362</v>
+      </c>
+      <c r="C43" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>372</v>
+      </c>
+      <c r="B44" t="s">
+        <v>362</v>
+      </c>
+      <c r="C44" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>372</v>
+      </c>
+      <c r="B45" t="s">
+        <v>362</v>
+      </c>
+      <c r="C45" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
+        <v>372</v>
+      </c>
+      <c r="B46" t="s">
+        <v>362</v>
+      </c>
+      <c r="C46" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>372</v>
+      </c>
+      <c r="B47" t="s">
+        <v>362</v>
+      </c>
+      <c r="C47" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>372</v>
+      </c>
+      <c r="B48" t="s">
+        <v>363</v>
+      </c>
+      <c r="C48" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" t="s">
+        <v>372</v>
+      </c>
+      <c r="B49" t="s">
+        <v>363</v>
+      </c>
+      <c r="C49" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" t="s">
+        <v>372</v>
+      </c>
+      <c r="B50" t="s">
+        <v>363</v>
+      </c>
+      <c r="C50" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" t="s">
+        <v>372</v>
+      </c>
+      <c r="B51" t="s">
+        <v>363</v>
+      </c>
+      <c r="C51" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" t="s">
+        <v>372</v>
+      </c>
+      <c r="B52" t="s">
+        <v>363</v>
+      </c>
+      <c r="C52" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" t="s">
+        <v>372</v>
+      </c>
+      <c r="B53" t="s">
+        <v>363</v>
+      </c>
+      <c r="C53" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" t="s">
+        <v>372</v>
+      </c>
+      <c r="B54" t="s">
+        <v>363</v>
+      </c>
+      <c r="C54" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" t="s">
+        <v>372</v>
+      </c>
+      <c r="B55" t="s">
+        <v>363</v>
+      </c>
+      <c r="C55" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" t="s">
+        <v>372</v>
+      </c>
+      <c r="B56" t="s">
+        <v>363</v>
+      </c>
+      <c r="C56" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" t="s">
+        <v>372</v>
+      </c>
+      <c r="B57" t="s">
+        <v>363</v>
+      </c>
+      <c r="C57" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" t="s">
+        <v>372</v>
+      </c>
+      <c r="B58" t="s">
+        <v>363</v>
+      </c>
+      <c r="C58" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" t="s">
+        <v>372</v>
+      </c>
+      <c r="B59" t="s">
+        <v>367</v>
+      </c>
+      <c r="C59" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" t="s">
+        <v>372</v>
+      </c>
+      <c r="B60" t="s">
+        <v>364</v>
+      </c>
+      <c r="C60" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" t="s">
+        <v>372</v>
+      </c>
+      <c r="B61" t="s">
+        <v>364</v>
+      </c>
+      <c r="C61" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" t="s">
+        <v>372</v>
+      </c>
+      <c r="B62" t="s">
+        <v>364</v>
+      </c>
+      <c r="C62" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" t="s">
+        <v>372</v>
+      </c>
+      <c r="B63" t="s">
+        <v>364</v>
+      </c>
+      <c r="C63" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" t="s">
+        <v>372</v>
+      </c>
+      <c r="B64" t="s">
+        <v>364</v>
+      </c>
+      <c r="C64" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" t="s">
+        <v>372</v>
+      </c>
+      <c r="B65" t="s">
+        <v>364</v>
+      </c>
+      <c r="C65" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" t="s">
+        <v>372</v>
+      </c>
+      <c r="B66" t="s">
+        <v>364</v>
+      </c>
+      <c r="C66" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" t="s">
+        <v>372</v>
+      </c>
+      <c r="B67" t="s">
+        <v>364</v>
+      </c>
+      <c r="C67" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" t="s">
+        <v>372</v>
+      </c>
+      <c r="B68" t="s">
+        <v>364</v>
+      </c>
+      <c r="C68" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" t="s">
+        <v>372</v>
+      </c>
+      <c r="B69" t="s">
+        <v>364</v>
+      </c>
+      <c r="C69" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" t="s">
+        <v>372</v>
+      </c>
+      <c r="B70" t="s">
+        <v>364</v>
+      </c>
+      <c r="C70" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" t="s">
+        <v>372</v>
+      </c>
+      <c r="B71" t="s">
+        <v>364</v>
+      </c>
+      <c r="C71" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" t="s">
+        <v>372</v>
+      </c>
+      <c r="B72" t="s">
+        <v>364</v>
+      </c>
+      <c r="C72" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" t="s">
+        <v>372</v>
+      </c>
+      <c r="B73" t="s">
+        <v>364</v>
+      </c>
+      <c r="C73" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" t="s">
+        <v>372</v>
+      </c>
+      <c r="B74" t="s">
+        <v>364</v>
+      </c>
+      <c r="C74" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" t="s">
+        <v>372</v>
+      </c>
+      <c r="B75" t="s">
+        <v>364</v>
+      </c>
+      <c r="C75" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" t="s">
+        <v>384</v>
+      </c>
+      <c r="B76" t="s">
+        <v>362</v>
+      </c>
+      <c r="C76" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" t="s">
+        <v>384</v>
+      </c>
+      <c r="B77" t="s">
+        <v>362</v>
+      </c>
+      <c r="C77" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" t="s">
+        <v>384</v>
+      </c>
+      <c r="B78" t="s">
+        <v>362</v>
+      </c>
+      <c r="C78" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" t="s">
+        <v>384</v>
+      </c>
+      <c r="B79" t="s">
+        <v>364</v>
+      </c>
+      <c r="C79" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" t="s">
+        <v>384</v>
+      </c>
+      <c r="B80" t="s">
+        <v>364</v>
+      </c>
+      <c r="C80" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" t="s">
+        <v>384</v>
+      </c>
+      <c r="B81" t="s">
+        <v>364</v>
+      </c>
+      <c r="C81" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" t="s">
+        <v>384</v>
+      </c>
+      <c r="B82" t="s">
+        <v>364</v>
+      </c>
+      <c r="C82" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" t="s">
+        <v>384</v>
+      </c>
+      <c r="B83" t="s">
+        <v>364</v>
+      </c>
+      <c r="C83" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" t="s">
+        <v>393</v>
+      </c>
+      <c r="B84" t="s">
+        <v>362</v>
+      </c>
+      <c r="C84" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" t="s">
+        <v>393</v>
+      </c>
+      <c r="B85" t="s">
+        <v>362</v>
+      </c>
+      <c r="C85" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" t="s">
+        <v>393</v>
+      </c>
+      <c r="B86" t="s">
+        <v>362</v>
+      </c>
+      <c r="C86" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" t="s">
+        <v>393</v>
+      </c>
+      <c r="B87" t="s">
+        <v>362</v>
+      </c>
+      <c r="C87" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88" t="s">
+        <v>393</v>
+      </c>
+      <c r="B88" t="s">
+        <v>363</v>
+      </c>
+      <c r="C88" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" t="s">
+        <v>393</v>
+      </c>
+      <c r="B89" t="s">
+        <v>363</v>
+      </c>
+      <c r="C89" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" t="s">
+        <v>393</v>
+      </c>
+      <c r="B90" t="s">
+        <v>363</v>
+      </c>
+      <c r="C90" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" t="s">
+        <v>393</v>
+      </c>
+      <c r="B91" t="s">
+        <v>363</v>
+      </c>
+      <c r="C91" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" t="s">
+        <v>393</v>
+      </c>
+      <c r="B92" t="s">
+        <v>363</v>
+      </c>
+      <c r="C92" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" t="s">
+        <v>393</v>
+      </c>
+      <c r="B93" t="s">
+        <v>363</v>
+      </c>
+      <c r="C93" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" t="s">
+        <v>393</v>
+      </c>
+      <c r="B94" t="s">
+        <v>363</v>
+      </c>
+      <c r="C94" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" t="s">
+        <v>393</v>
+      </c>
+      <c r="B95" t="s">
+        <v>363</v>
+      </c>
+      <c r="C95" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" t="s">
+        <v>393</v>
+      </c>
+      <c r="B96" t="s">
+        <v>363</v>
+      </c>
+      <c r="C96" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" t="s">
+        <v>393</v>
+      </c>
+      <c r="B97" t="s">
+        <v>363</v>
+      </c>
+      <c r="C97" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" t="s">
+        <v>393</v>
+      </c>
+      <c r="B98" t="s">
+        <v>363</v>
+      </c>
+      <c r="C98" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" t="s">
+        <v>393</v>
+      </c>
+      <c r="B99" t="s">
+        <v>363</v>
+      </c>
+      <c r="C99" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" t="s">
+        <v>393</v>
+      </c>
+      <c r="B100" t="s">
+        <v>363</v>
+      </c>
+      <c r="C100" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101" t="s">
+        <v>393</v>
+      </c>
+      <c r="B101" t="s">
+        <v>363</v>
+      </c>
+      <c r="C101" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102" t="s">
+        <v>393</v>
+      </c>
+      <c r="B102" t="s">
+        <v>363</v>
+      </c>
+      <c r="C102" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103" t="s">
+        <v>393</v>
+      </c>
+      <c r="B103" t="s">
+        <v>369</v>
+      </c>
+      <c r="C103" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104" t="s">
+        <v>393</v>
+      </c>
+      <c r="B104" t="s">
+        <v>369</v>
+      </c>
+      <c r="C104" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105" t="s">
+        <v>393</v>
+      </c>
+      <c r="B105" t="s">
+        <v>364</v>
+      </c>
+      <c r="C105" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106" t="s">
+        <v>393</v>
+      </c>
+      <c r="B106" t="s">
+        <v>371</v>
+      </c>
+      <c r="C106" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107" t="s">
+        <v>393</v>
+      </c>
+      <c r="B107" t="s">
+        <v>371</v>
+      </c>
+      <c r="C107" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108" t="s">
+        <v>409</v>
+      </c>
+      <c r="B108" t="s">
+        <v>362</v>
+      </c>
+      <c r="C108" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109" t="s">
+        <v>409</v>
+      </c>
+      <c r="B109" t="s">
+        <v>362</v>
+      </c>
+      <c r="C109" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110" t="s">
+        <v>409</v>
+      </c>
+      <c r="B110" t="s">
+        <v>362</v>
+      </c>
+      <c r="C110" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111" t="s">
+        <v>409</v>
+      </c>
+      <c r="B111" t="s">
+        <v>362</v>
+      </c>
+      <c r="C111" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A112" t="s">
+        <v>409</v>
+      </c>
+      <c r="B112" t="s">
+        <v>362</v>
+      </c>
+      <c r="C112" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113" t="s">
+        <v>409</v>
+      </c>
+      <c r="B113" t="s">
+        <v>362</v>
+      </c>
+      <c r="C113" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114" t="s">
+        <v>409</v>
+      </c>
+      <c r="B114" t="s">
+        <v>363</v>
+      </c>
+      <c r="C114" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115" t="s">
+        <v>409</v>
+      </c>
+      <c r="B115" t="s">
+        <v>363</v>
+      </c>
+      <c r="C115" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A116" t="s">
+        <v>409</v>
+      </c>
+      <c r="B116" t="s">
+        <v>363</v>
+      </c>
+      <c r="C116" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117" t="s">
+        <v>409</v>
+      </c>
+      <c r="B117" t="s">
+        <v>363</v>
+      </c>
+      <c r="C117" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A118" t="s">
+        <v>409</v>
+      </c>
+      <c r="B118" t="s">
+        <v>363</v>
+      </c>
+      <c r="C118" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A119" t="s">
+        <v>409</v>
+      </c>
+      <c r="B119" t="s">
+        <v>369</v>
+      </c>
+      <c r="C119" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A120" t="s">
+        <v>409</v>
+      </c>
+      <c r="B120" t="s">
+        <v>367</v>
+      </c>
+      <c r="C120" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A121" t="s">
+        <v>409</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C121" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A122" t="s">
+        <v>409</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C122" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A123" t="s">
+        <v>409</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C123" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A124" t="s">
+        <v>409</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C124" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A125" t="s">
+        <v>409</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A126" t="s">
+        <v>390</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C126" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A127" t="s">
+        <v>390</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C127" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A128" t="s">
+        <v>390</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C128" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A129" t="s">
+        <v>390</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C129" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A130" t="s">
+        <v>390</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C130" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A131" t="s">
+        <v>390</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C131" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A132" t="s">
+        <v>390</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C132" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A133" t="s">
+        <v>390</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C133" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A134" t="s">
+        <v>390</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C134" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A135" t="s">
+        <v>390</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C135" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A136" t="s">
+        <v>390</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C136" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A137" t="s">
+        <v>390</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C137" t="s">
+        <v>426</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>